<commit_message>
more work on report
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="backlog" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="88">
   <si>
     <t>Description</t>
   </si>
@@ -292,6 +292,15 @@
   </si>
   <si>
     <t>Retard</t>
+  </si>
+  <si>
+    <t>Données / PIM / GT</t>
+  </si>
+  <si>
+    <t>Insérer en annexe la ground truth. Attention, il y a des soucis d'encodage, c'est assez pénible. (cf. notebook ground_truth)</t>
+  </si>
+  <si>
+    <t>Terminé</t>
   </si>
 </sst>
 </file>
@@ -636,7 +645,7 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>#N/A</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>#N/A</c:v>
@@ -663,11 +672,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="389835368"/>
-        <c:axId val="389840464"/>
+        <c:axId val="124708720"/>
+        <c:axId val="124709112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="389835368"/>
+        <c:axId val="124708720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -724,12 +733,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389840464"/>
+        <c:crossAx val="124709112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="389840464"/>
+        <c:axId val="124709112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -786,7 +795,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="389835368"/>
+        <c:crossAx val="124708720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1691,9 +1700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:H147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+    <sheetView zoomScale="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1715,7 +1724,7 @@
       <c r="D1" s="20"/>
       <c r="E1" s="4">
         <f>SUM(E5:E396)</f>
-        <v>276</v>
+        <v>279</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
@@ -1827,9 +1836,11 @@
       </c>
       <c r="G7" s="15" t="str">
         <f t="shared" ref="G7:G68" si="0">IF(ISBLANK(H7),"A faire","Terminé")</f>
-        <v>A faire</v>
-      </c>
-      <c r="H7" s="15"/>
+        <v>Terminé</v>
+      </c>
+      <c r="H7" s="16">
+        <v>43954</v>
+      </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
@@ -1849,9 +1860,11 @@
       </c>
       <c r="G8" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>A faire</v>
-      </c>
-      <c r="H8" s="15"/>
+        <v>Terminé</v>
+      </c>
+      <c r="H8" s="16">
+        <v>43954</v>
+      </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
@@ -1871,9 +1884,11 @@
       </c>
       <c r="G9" s="15" t="str">
         <f t="shared" si="0"/>
-        <v>A faire</v>
-      </c>
-      <c r="H9" s="16"/>
+        <v>Terminé</v>
+      </c>
+      <c r="H9" s="16">
+        <v>43954</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
@@ -1891,11 +1906,12 @@
       <c r="F10" s="15">
         <v>1</v>
       </c>
-      <c r="G10" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v>A faire</v>
-      </c>
-      <c r="H10" s="15"/>
+      <c r="G10" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="16">
+        <v>43954</v>
+      </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
@@ -2820,10 +2836,18 @@
       <c r="H55" s="12"/>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="12"/>
-      <c r="C56" s="12"/>
-      <c r="D56" s="11"/>
-      <c r="E56" s="12"/>
+      <c r="B56" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D56" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E56" s="12">
+        <v>3</v>
+      </c>
       <c r="F56" s="12"/>
       <c r="G56" s="12" t="str">
         <f t="shared" si="0"/>
@@ -3936,8 +3960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3960,7 +3984,7 @@
       </c>
       <c r="F2" s="17">
         <f ca="1">TODAY()</f>
-        <v>43953</v>
+        <v>43954</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4012,9 +4036,9 @@
         <f ca="1">IF($F$2&gt;=D$5,SUMPRODUCT(--(backlog!$E$4:$E$147),--(backlog!$F$4:$F$147=1),--(backlog!$H$4:$H$147&lt;=Burndown!D$5),--(backlog!$G$4:$G$147="Terminé")),NA())</f>
         <v>10</v>
       </c>
-      <c r="E6" s="3" t="e">
+      <c r="E6" s="3">
         <f ca="1">IF($F$2&gt;=E$5,SUMPRODUCT(--(backlog!$E$4:$E$147),--(backlog!$F$4:$F$147=1),--(backlog!$H$4:$H$147&lt;=Burndown!E$5),--(backlog!$G$4:$G$147="Terminé")),NA())</f>
-        <v>#N/A</v>
+        <v>21</v>
       </c>
       <c r="F6" s="3" t="e">
         <f ca="1">IF($F$2&gt;=F$5,SUMPRODUCT(--(backlog!$E$4:$E$147),--(backlog!$F$4:$F$147=1),--(backlog!$H$4:$H$147&lt;=Burndown!F$5),--(backlog!$G$4:$G$147="Terminé")),NA())</f>
@@ -4049,9 +4073,9 @@
         <f t="shared" ref="D7:I7" ca="1" si="0">IF($F$2&gt;=D$5,$B$2-D6,NA())</f>
         <v>67</v>
       </c>
-      <c r="E7" s="3" t="e">
+      <c r="E7" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>#N/A</v>
+        <v>56</v>
       </c>
       <c r="F7" s="3" t="e">
         <f t="shared" ca="1" si="0"/>
@@ -4123,9 +4147,9 @@
         <f t="shared" ca="1" si="1"/>
         <v>-12</v>
       </c>
-      <c r="E9" s="3" t="e">
+      <c r="E9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>#N/A</v>
+        <v>-12</v>
       </c>
       <c r="F9" s="3" t="e">
         <f t="shared" ca="1" si="1"/>

</xml_diff>

<commit_message>
new version after first check
</commit_message>
<xml_diff>
--- a/backlog.xlsx
+++ b/backlog.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="166">
   <si>
     <t>Description</t>
   </si>
@@ -601,6 +601,9 @@
 model_tuning : OK
 open_model : OK
 Performance_measurement : OK</t>
+  </si>
+  <si>
+    <t>Attention ! &lt;rien&gt; &lt;rien&gt; donne une similarité à 0 % dans l'évaluation de la performance.</t>
   </si>
 </sst>
 </file>
@@ -1170,11 +1173,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385531424"/>
-        <c:axId val="385530248"/>
+        <c:axId val="388160312"/>
+        <c:axId val="388155216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385531424"/>
+        <c:axId val="388160312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1231,12 +1234,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385530248"/>
+        <c:crossAx val="388155216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385530248"/>
+        <c:axId val="388155216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1293,7 +1296,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385531424"/>
+        <c:crossAx val="388160312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1558,11 +1561,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385530640"/>
-        <c:axId val="385528680"/>
+        <c:axId val="388156784"/>
+        <c:axId val="388157176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385530640"/>
+        <c:axId val="388156784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1619,12 +1622,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385528680"/>
+        <c:crossAx val="388157176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385528680"/>
+        <c:axId val="388157176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1681,7 +1684,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385530640"/>
+        <c:crossAx val="388156784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1946,11 +1949,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385525152"/>
-        <c:axId val="385525544"/>
+        <c:axId val="388157960"/>
+        <c:axId val="387078144"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385525152"/>
+        <c:axId val="388157960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,12 +2010,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385525544"/>
+        <c:crossAx val="387078144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385525544"/>
+        <c:axId val="387078144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2069,7 +2072,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385525152"/>
+        <c:crossAx val="388157960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4148,14 +4151,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="B1:H156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B32" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B98" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="D78" sqref="D78"/>
+      <selection pane="bottomRight" activeCell="D101" sqref="D101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4230,7 +4232,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="2:8" s="17" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
         <v>10</v>
       </c>
@@ -4254,7 +4256,7 @@
         <v>43953</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
@@ -4278,7 +4280,7 @@
         <v>43952</v>
       </c>
     </row>
-    <row r="7" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="13" t="s">
         <v>10</v>
       </c>
@@ -4302,7 +4304,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="8" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
@@ -4326,7 +4328,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="9" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>10</v>
       </c>
@@ -4350,7 +4352,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="10" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>10</v>
       </c>
@@ -4373,7 +4375,7 @@
         <v>43954</v>
       </c>
     </row>
-    <row r="11" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>10</v>
       </c>
@@ -4397,7 +4399,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="12" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
@@ -4421,7 +4423,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="13" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
@@ -4445,7 +4447,7 @@
         <v>43959</v>
       </c>
     </row>
-    <row r="14" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>10</v>
       </c>
@@ -4469,7 +4471,7 @@
         <v>43960</v>
       </c>
     </row>
-    <row r="15" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>10</v>
       </c>
@@ -4493,7 +4495,7 @@
         <v>43962</v>
       </c>
     </row>
-    <row r="16" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>10</v>
       </c>
@@ -4517,7 +4519,7 @@
         <v>43962</v>
       </c>
     </row>
-    <row r="17" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>10</v>
       </c>
@@ -4541,7 +4543,7 @@
         <v>43963</v>
       </c>
     </row>
-    <row r="18" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>10</v>
       </c>
@@ -4565,7 +4567,7 @@
         <v>43963</v>
       </c>
     </row>
-    <row r="19" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>10</v>
       </c>
@@ -4589,7 +4591,7 @@
         <v>43964</v>
       </c>
     </row>
-    <row r="20" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>10</v>
       </c>
@@ -4613,7 +4615,7 @@
         <v>43963</v>
       </c>
     </row>
-    <row r="21" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>10</v>
       </c>
@@ -4637,7 +4639,7 @@
         <v>43955</v>
       </c>
     </row>
-    <row r="22" spans="2:8" s="17" customFormat="1" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" s="17" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
         <v>10</v>
       </c>
@@ -4661,7 +4663,7 @@
         <v>43956</v>
       </c>
     </row>
-    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="11" t="s">
         <v>10</v>
       </c>
@@ -4685,7 +4687,7 @@
         <v>43964</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>10</v>
       </c>
@@ -4709,7 +4711,7 @@
         <v>43966</v>
       </c>
     </row>
-    <row r="25" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="11" t="s">
         <v>10</v>
       </c>
@@ -4733,7 +4735,7 @@
         <v>43969</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>10</v>
       </c>
@@ -4757,7 +4759,7 @@
         <v>43966</v>
       </c>
     </row>
-    <row r="27" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>10</v>
       </c>
@@ -4781,7 +4783,7 @@
         <v>43970</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B28" s="11" t="s">
         <v>10</v>
       </c>
@@ -4805,7 +4807,7 @@
         <v>43969</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>10</v>
       </c>
@@ -4829,7 +4831,7 @@
         <v>43967</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>10</v>
       </c>
@@ -4915,7 +4917,7 @@
       </c>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
         <v>9</v>
       </c>
@@ -4939,7 +4941,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>9</v>
       </c>
@@ -4963,7 +4965,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>9</v>
       </c>
@@ -4987,7 +4989,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="36.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="11" t="s">
         <v>10</v>
       </c>
@@ -5033,7 +5035,7 @@
         <v>43989</v>
       </c>
     </row>
-    <row r="39" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
         <v>10</v>
       </c>
@@ -5052,7 +5054,7 @@
       </c>
       <c r="H39" s="15"/>
     </row>
-    <row r="40" spans="2:8" s="17" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="s">
         <v>58</v>
       </c>
@@ -5071,7 +5073,7 @@
       </c>
       <c r="H40" s="15"/>
     </row>
-    <row r="41" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>10</v>
       </c>
@@ -5095,7 +5097,7 @@
         <v>43957</v>
       </c>
     </row>
-    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>9</v>
       </c>
@@ -5139,7 +5141,7 @@
       </c>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>10</v>
       </c>
@@ -5158,7 +5160,7 @@
       </c>
       <c r="H44" s="11"/>
     </row>
-    <row r="45" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="11" t="s">
         <v>58</v>
       </c>
@@ -5180,7 +5182,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="46" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="11" t="s">
         <v>58</v>
       </c>
@@ -5202,7 +5204,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="11" t="s">
         <v>10</v>
       </c>
@@ -5224,7 +5226,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="11" t="s">
         <v>10</v>
       </c>
@@ -5246,7 +5248,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="11" t="s">
         <v>10</v>
       </c>
@@ -5268,7 +5270,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="50" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
         <v>10</v>
       </c>
@@ -5287,7 +5289,7 @@
       </c>
       <c r="H50" s="11"/>
     </row>
-    <row r="51" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
         <v>10</v>
       </c>
@@ -5306,7 +5308,7 @@
       </c>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="9" t="s">
         <v>10</v>
       </c>
@@ -5325,7 +5327,7 @@
       </c>
       <c r="H52" s="11"/>
     </row>
-    <row r="53" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
         <v>9</v>
       </c>
@@ -5344,7 +5346,7 @@
       </c>
       <c r="H53" s="11"/>
     </row>
-    <row r="54" spans="2:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B54" s="9" t="s">
         <v>10</v>
       </c>
@@ -5363,7 +5365,7 @@
       </c>
       <c r="H54" s="12"/>
     </row>
-    <row r="55" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="9" t="s">
         <v>10</v>
       </c>
@@ -5382,7 +5384,7 @@
       </c>
       <c r="H55" s="11"/>
     </row>
-    <row r="56" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
         <v>10</v>
       </c>
@@ -5401,7 +5403,7 @@
       </c>
       <c r="H56" s="11"/>
     </row>
-    <row r="57" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
         <v>9</v>
       </c>
@@ -5420,7 +5422,7 @@
       </c>
       <c r="H57" s="11"/>
     </row>
-    <row r="58" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
         <v>10</v>
       </c>
@@ -5439,7 +5441,7 @@
       </c>
       <c r="H58" s="11"/>
     </row>
-    <row r="59" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="11" t="s">
         <v>10</v>
       </c>
@@ -5458,7 +5460,7 @@
       </c>
       <c r="H59" s="11"/>
     </row>
-    <row r="60" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="11" t="s">
         <v>10</v>
       </c>
@@ -5477,7 +5479,7 @@
       </c>
       <c r="H60" s="11"/>
     </row>
-    <row r="61" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="11" t="s">
         <v>10</v>
       </c>
@@ -5496,7 +5498,7 @@
       </c>
       <c r="H61" s="11"/>
     </row>
-    <row r="62" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="11" t="s">
         <v>10</v>
       </c>
@@ -5515,7 +5517,7 @@
       </c>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B63" s="11" t="s">
         <v>10</v>
       </c>
@@ -5534,7 +5536,7 @@
       </c>
       <c r="H63" s="11"/>
     </row>
-    <row r="64" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B64" s="11" t="s">
         <v>10</v>
       </c>
@@ -5633,7 +5635,7 @@
       </c>
       <c r="H68" s="11"/>
     </row>
-    <row r="69" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B69" s="11" t="s">
         <v>10</v>
       </c>
@@ -5652,7 +5654,7 @@
       </c>
       <c r="H69" s="11"/>
     </row>
-    <row r="70" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="11" t="s">
         <v>10</v>
       </c>
@@ -5671,7 +5673,7 @@
       </c>
       <c r="H70" s="11"/>
     </row>
-    <row r="71" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="11" t="s">
         <v>10</v>
       </c>
@@ -5710,7 +5712,7 @@
       </c>
       <c r="H72" s="11"/>
     </row>
-    <row r="73" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="11" t="s">
         <v>10</v>
       </c>
@@ -5729,7 +5731,7 @@
       </c>
       <c r="H73" s="11"/>
     </row>
-    <row r="74" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B74" s="11" t="s">
         <v>10</v>
       </c>
@@ -5771,7 +5773,7 @@
       </c>
       <c r="H75" s="11"/>
     </row>
-    <row r="76" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="11" t="s">
         <v>9</v>
       </c>
@@ -5793,7 +5795,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="77" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="11" t="s">
         <v>9</v>
       </c>
@@ -5855,7 +5857,7 @@
       </c>
       <c r="H79" s="11"/>
     </row>
-    <row r="80" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="11" t="s">
         <v>9</v>
       </c>
@@ -5877,7 +5879,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="81" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B81" s="11" t="s">
         <v>10</v>
       </c>
@@ -5899,7 +5901,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="82" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="11" t="s">
         <v>10</v>
       </c>
@@ -5918,7 +5920,7 @@
       </c>
       <c r="H82" s="11"/>
     </row>
-    <row r="83" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="11" t="s">
         <v>10</v>
       </c>
@@ -5937,7 +5939,7 @@
       </c>
       <c r="H83" s="11"/>
     </row>
-    <row r="84" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="11" t="s">
         <v>10</v>
       </c>
@@ -5959,7 +5961,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="85" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B85" s="11" t="s">
         <v>10</v>
       </c>
@@ -5981,7 +5983,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="86" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B86" s="11" t="s">
         <v>9</v>
       </c>
@@ -6023,7 +6025,7 @@
       </c>
       <c r="H87" s="11"/>
     </row>
-    <row r="88" spans="2:8" ht="48" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B88" s="11" t="s">
         <v>126</v>
       </c>
@@ -6045,7 +6047,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="89" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="11" t="s">
         <v>58</v>
       </c>
@@ -6064,7 +6066,7 @@
       </c>
       <c r="H89" s="11"/>
     </row>
-    <row r="90" spans="2:8" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B90" s="11" t="s">
         <v>126</v>
       </c>
@@ -6106,7 +6108,7 @@
       </c>
       <c r="H91" s="11"/>
     </row>
-    <row r="92" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="11" t="s">
         <v>10</v>
       </c>
@@ -6125,7 +6127,7 @@
       </c>
       <c r="H92" s="11"/>
     </row>
-    <row r="93" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="11" t="s">
         <v>10</v>
       </c>
@@ -6144,7 +6146,7 @@
       </c>
       <c r="H93" s="11"/>
     </row>
-    <row r="94" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B94" s="11" t="s">
         <v>10</v>
       </c>
@@ -6168,7 +6170,7 @@
         <v>43967</v>
       </c>
     </row>
-    <row r="95" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="11" t="s">
         <v>10</v>
       </c>
@@ -6190,7 +6192,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="96" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="11" t="s">
         <v>10</v>
       </c>
@@ -6209,7 +6211,7 @@
       </c>
       <c r="H96" s="11"/>
     </row>
-    <row r="97" spans="2:8" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B97" s="11" t="s">
         <v>130</v>
       </c>
@@ -6229,7 +6231,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="98" spans="2:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B98" s="11" t="s">
         <v>130</v>
       </c>
@@ -6249,7 +6251,7 @@
         <v>43988</v>
       </c>
     </row>
-    <row r="99" spans="2:8" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="11" t="s">
         <v>130</v>
       </c>
@@ -6272,7 +6274,9 @@
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="11"/>
       <c r="C100" s="11"/>
-      <c r="D100" s="10"/>
+      <c r="D100" s="10" t="s">
+        <v>165</v>
+      </c>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
       <c r="G100" s="11" t="str">
@@ -6954,13 +6958,7 @@
       <c r="H156" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:H156">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="A faire"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B3:H156"/>
   <mergeCells count="1">
     <mergeCell ref="B1:D1"/>
   </mergeCells>
@@ -7090,7 +7088,7 @@
       </c>
       <c r="H5" s="32">
         <f ca="1">TODAY()</f>
-        <v>43990</v>
+        <v>43993</v>
       </c>
       <c r="I5" s="22"/>
       <c r="J5" s="22"/>
@@ -8080,7 +8078,7 @@
       </c>
       <c r="H64" s="32">
         <f ca="1">TODAY()</f>
-        <v>43990</v>
+        <v>43993</v>
       </c>
       <c r="I64" s="22"/>
       <c r="J64" s="22"/>

</xml_diff>